<commit_message>
notes on test data
</commit_message>
<xml_diff>
--- a/taxonomy_pipeline/test_data/bayes_idtax_lca_pr2_mapped.xlsx
+++ b/taxonomy_pipeline/test_data/bayes_idtax_lca_pr2_mapped.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thecomplexgeek/Desktop/Taxonomic Sequencing/amplicon_bioinformatics/taxonomy_pipeline/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5CCB0-537A-1A41-9784-CC6127BD4137}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F9DA96-C7D2-8A46-B3C2-544CA5C2C347}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="700" windowWidth="28040" windowHeight="17300" xr2:uid="{EDC9F8DD-534D-7544-B7B8-44B7608BA464}"/>
+    <workbookView xWindow="1600" yWindow="2880" windowWidth="25420" windowHeight="12920" xr2:uid="{EDC9F8DD-534D-7544-B7B8-44B7608BA464}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="222">
   <si>
     <t>Bayes</t>
   </si>
@@ -685,6 +685,18 @@
   </si>
   <si>
     <t>RESULT</t>
+  </si>
+  <si>
+    <t>NA (Eukaryota if no NA as name)</t>
+  </si>
+  <si>
+    <t>ties -&gt; grab the one that user defined</t>
+  </si>
+  <si>
+    <t>make sure the table name lines up with the table name</t>
+  </si>
+  <si>
+    <t>automatic tie breaker -&gt; NA</t>
   </si>
 </sst>
 </file>
@@ -1036,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83AF2A6-2E24-F146-8FBC-B9849A546C26}">
-  <dimension ref="A2:L191"/>
+  <dimension ref="A2:M191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P185" sqref="P185"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="138" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1787,7 +1799,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1822,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>22</v>
       </c>
@@ -1851,7 +1863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>22</v>
       </c>
@@ -1880,7 +1892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>22</v>
       </c>
@@ -1909,7 +1921,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1944,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
         <v>22</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>14</v>
       </c>
@@ -2002,7 +2014,28 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>218</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" t="s">
+        <v>14</v>
+      </c>
       <c r="K41" t="s">
         <v>14</v>
       </c>
@@ -2010,7 +2043,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -2045,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
         <v>22</v>
       </c>
@@ -2074,7 +2107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
         <v>14</v>
       </c>
@@ -2103,7 +2136,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" t="s">
+        <v>14</v>
+      </c>
       <c r="I46" t="s">
         <v>14</v>
       </c>
@@ -2117,7 +2165,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -2151,8 +2199,11 @@
       <c r="L48" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
         <v>22</v>
       </c>
@@ -2180,8 +2231,11 @@
       <c r="L49" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
         <v>22</v>
       </c>
@@ -2210,7 +2264,28 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" t="s">
+        <v>69</v>
+      </c>
+      <c r="G51" t="s">
+        <v>70</v>
+      </c>
+      <c r="H51" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" t="s">
+        <v>14</v>
+      </c>
       <c r="K51" t="s">
         <v>14</v>
       </c>
@@ -2218,7 +2293,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -2253,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D54" t="s">
         <v>22</v>
       </c>
@@ -2282,7 +2357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
         <v>22</v>
       </c>
@@ -2311,7 +2386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D56" t="s">
         <v>22</v>
       </c>
@@ -2340,7 +2415,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>92</v>
       </c>
@@ -2375,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
         <v>22</v>
       </c>
@@ -2404,7 +2479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
         <v>14</v>
       </c>
@@ -2433,7 +2508,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" t="s">
+        <v>14</v>
+      </c>
       <c r="J61" t="s">
         <v>14</v>
       </c>
@@ -2444,7 +2537,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>101</v>
       </c>
@@ -2478,8 +2571,11 @@
       <c r="L63" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D64" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
validate with test data
</commit_message>
<xml_diff>
--- a/taxonomy_pipeline/test_data/bayes_idtax_lca_pr2_mapped.xlsx
+++ b/taxonomy_pipeline/test_data/bayes_idtax_lca_pr2_mapped.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thecomplexgeek/Desktop/Taxonomic Sequencing/amplicon_bioinformatics/taxonomy_pipeline/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F9DA96-C7D2-8A46-B3C2-544CA5C2C347}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D667EB4-FC71-804B-A411-D34CC81CA5C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="2880" windowWidth="25420" windowHeight="12920" xr2:uid="{EDC9F8DD-534D-7544-B7B8-44B7608BA464}"/>
+    <workbookView xWindow="1640" yWindow="2100" windowWidth="25420" windowHeight="12920" xr2:uid="{EDC9F8DD-534D-7544-B7B8-44B7608BA464}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="222">
   <si>
     <t>Bayes</t>
   </si>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83AF2A6-2E24-F146-8FBC-B9849A546C26}">
   <dimension ref="A2:M191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="138" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="F195" sqref="F195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2634,6 +2634,21 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" t="s">
+        <v>68</v>
+      </c>
+      <c r="F66" t="s">
+        <v>85</v>
+      </c>
+      <c r="G66" t="s">
+        <v>86</v>
+      </c>
+      <c r="H66" t="s">
+        <v>14</v>
+      </c>
       <c r="I66" t="s">
         <v>14</v>
       </c>
@@ -3104,6 +3119,27 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" t="s">
+        <v>68</v>
+      </c>
+      <c r="F86" t="s">
+        <v>85</v>
+      </c>
+      <c r="G86" t="s">
+        <v>118</v>
+      </c>
+      <c r="H86" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" t="s">
+        <v>14</v>
+      </c>
+      <c r="J86" t="s">
+        <v>14</v>
+      </c>
       <c r="K86" t="s">
         <v>14</v>
       </c>
@@ -3205,6 +3241,9 @@
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>14</v>
+      </c>
       <c r="E91" t="s">
         <v>14</v>
       </c>
@@ -3934,6 +3973,27 @@
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" t="s">
+        <v>14</v>
+      </c>
+      <c r="G121" t="s">
+        <v>14</v>
+      </c>
+      <c r="H121" t="s">
+        <v>14</v>
+      </c>
+      <c r="I121" t="s">
+        <v>14</v>
+      </c>
+      <c r="J121" t="s">
+        <v>14</v>
+      </c>
       <c r="K121" t="s">
         <v>14</v>
       </c>
@@ -4157,6 +4217,24 @@
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>22</v>
+      </c>
+      <c r="E131" t="s">
+        <v>43</v>
+      </c>
+      <c r="F131" t="s">
+        <v>44</v>
+      </c>
+      <c r="G131" t="s">
+        <v>129</v>
+      </c>
+      <c r="H131" t="s">
+        <v>14</v>
+      </c>
+      <c r="I131" t="s">
+        <v>14</v>
+      </c>
       <c r="J131" t="s">
         <v>14</v>
       </c>
@@ -4261,6 +4339,18 @@
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>22</v>
+      </c>
+      <c r="E136" t="s">
+        <v>43</v>
+      </c>
+      <c r="F136" t="s">
+        <v>44</v>
+      </c>
+      <c r="G136" t="s">
+        <v>14</v>
+      </c>
       <c r="H136" t="s">
         <v>14</v>
       </c>
@@ -4371,6 +4461,24 @@
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>22</v>
+      </c>
+      <c r="E141" t="s">
+        <v>43</v>
+      </c>
+      <c r="F141" t="s">
+        <v>44</v>
+      </c>
+      <c r="G141" t="s">
+        <v>129</v>
+      </c>
+      <c r="H141" t="s">
+        <v>14</v>
+      </c>
+      <c r="I141" t="s">
+        <v>14</v>
+      </c>
       <c r="J141" t="s">
         <v>14</v>
       </c>
@@ -4475,6 +4583,15 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>22</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146" t="s">
+        <v>14</v>
+      </c>
       <c r="G146" t="s">
         <v>14</v>
       </c>
@@ -4588,6 +4705,24 @@
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
+        <v>22</v>
+      </c>
+      <c r="E151" t="s">
+        <v>43</v>
+      </c>
+      <c r="F151" t="s">
+        <v>56</v>
+      </c>
+      <c r="G151" t="s">
+        <v>165</v>
+      </c>
+      <c r="H151" t="s">
+        <v>173</v>
+      </c>
+      <c r="I151" t="s">
+        <v>14</v>
+      </c>
       <c r="J151" t="s">
         <v>14</v>
       </c>
@@ -4814,6 +4949,21 @@
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D161" t="s">
+        <v>22</v>
+      </c>
+      <c r="E161" t="s">
+        <v>14</v>
+      </c>
+      <c r="F161" t="s">
+        <v>14</v>
+      </c>
+      <c r="G161" t="s">
+        <v>14</v>
+      </c>
+      <c r="H161" t="s">
+        <v>14</v>
+      </c>
       <c r="I161" t="s">
         <v>14</v>
       </c>
@@ -4921,6 +5071,27 @@
       </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D166" t="s">
+        <v>22</v>
+      </c>
+      <c r="E166" t="s">
+        <v>43</v>
+      </c>
+      <c r="F166" t="s">
+        <v>56</v>
+      </c>
+      <c r="G166" t="s">
+        <v>165</v>
+      </c>
+      <c r="H166" t="s">
+        <v>173</v>
+      </c>
+      <c r="I166" t="s">
+        <v>182</v>
+      </c>
+      <c r="J166" t="s">
+        <v>14</v>
+      </c>
       <c r="K166" t="s">
         <v>14</v>
       </c>
@@ -5022,6 +5193,27 @@
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
+        <v>22</v>
+      </c>
+      <c r="E171" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171" t="s">
+        <v>14</v>
+      </c>
+      <c r="G171" t="s">
+        <v>14</v>
+      </c>
+      <c r="H171" t="s">
+        <v>14</v>
+      </c>
+      <c r="I171" t="s">
+        <v>14</v>
+      </c>
+      <c r="J171" t="s">
+        <v>14</v>
+      </c>
       <c r="K171" t="s">
         <v>14</v>
       </c>
@@ -5367,6 +5559,30 @@
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D186" t="s">
+        <v>22</v>
+      </c>
+      <c r="E186" t="s">
+        <v>43</v>
+      </c>
+      <c r="F186" t="s">
+        <v>56</v>
+      </c>
+      <c r="G186" t="s">
+        <v>165</v>
+      </c>
+      <c r="H186" t="s">
+        <v>173</v>
+      </c>
+      <c r="I186" t="s">
+        <v>182</v>
+      </c>
+      <c r="J186" t="s">
+        <v>14</v>
+      </c>
+      <c r="K186" t="s">
+        <v>14</v>
+      </c>
       <c r="L186" t="s">
         <v>217</v>
       </c>
@@ -5465,6 +5681,27 @@
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D191" t="s">
+        <v>22</v>
+      </c>
+      <c r="E191" t="s">
+        <v>43</v>
+      </c>
+      <c r="F191" t="s">
+        <v>56</v>
+      </c>
+      <c r="G191" t="s">
+        <v>165</v>
+      </c>
+      <c r="H191" t="s">
+        <v>173</v>
+      </c>
+      <c r="I191" t="s">
+        <v>182</v>
+      </c>
+      <c r="J191" t="s">
+        <v>14</v>
+      </c>
       <c r="K191" t="s">
         <v>14</v>
       </c>

</xml_diff>